<commit_message>
CRUD wilayah(prov, kab, etc) & adding validation
</commit_message>
<xml_diff>
--- a/dokumentasi/Analisa New Webtool.xlsx
+++ b/dokumentasi/Analisa New Webtool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel" sheetId="1" state="visible" r:id="rId2"/>
@@ -558,7 +558,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.89"/>
@@ -733,7 +733,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.11"/>
@@ -910,11 +910,11 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.11"/>
@@ -1095,7 +1095,7 @@
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -1222,10 +1222,10 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -1483,7 +1483,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -1699,7 +1699,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -1917,14 +1917,14 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2185,10 +2185,10 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -2356,10 +2356,10 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -2525,11 +2525,11 @@
   </sheetPr>
   <dimension ref="A2:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.99"/>
@@ -2537,7 +2537,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
   <sheetData>
@@ -2735,7 +2735,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -2913,7 +2913,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -3114,7 +3114,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
@@ -3338,7 +3338,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>

</xml_diff>